<commit_message>
Make a change to the docs
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>A1</t>
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>C3</t>
   </si>
 </sst>
 </file>
@@ -381,22 +384,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make the Office files blank
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -24,20 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,35 +374,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the Office files for diff
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -24,7 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Hello, World!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,7 +383,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>